<commit_message>
Just ti keep it updated
</commit_message>
<xml_diff>
--- a/Diario de fusão.xlsx
+++ b/Diario de fusão.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C822"/>
+  <dimension ref="A1:C877"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10986,15 +10986,11 @@
           <t>14/05/2025</t>
         </is>
       </c>
-      <c r="B812" t="inlineStr">
-        <is>
-          <t>2811</t>
-        </is>
-      </c>
-      <c r="C812" t="inlineStr">
-        <is>
-          <t>650</t>
-        </is>
+      <c r="B812" t="n">
+        <v>2811</v>
+      </c>
+      <c r="C812" t="n">
+        <v>650</v>
       </c>
     </row>
     <row r="813">
@@ -11003,15 +10999,11 @@
           <t>14/05/2025</t>
         </is>
       </c>
-      <c r="B813" t="inlineStr">
-        <is>
-          <t>3581</t>
-        </is>
-      </c>
-      <c r="C813" t="inlineStr">
-        <is>
-          <t>457</t>
-        </is>
+      <c r="B813" t="n">
+        <v>3581</v>
+      </c>
+      <c r="C813" t="n">
+        <v>457</v>
       </c>
     </row>
     <row r="814">
@@ -11020,15 +11012,11 @@
           <t>14/05/2025</t>
         </is>
       </c>
-      <c r="B814" t="inlineStr">
-        <is>
-          <t>2651</t>
-        </is>
-      </c>
-      <c r="C814" t="inlineStr">
-        <is>
-          <t>135</t>
-        </is>
+      <c r="B814" t="n">
+        <v>2651</v>
+      </c>
+      <c r="C814" t="n">
+        <v>135</v>
       </c>
     </row>
     <row r="815">
@@ -11037,15 +11025,11 @@
           <t>14/05/2025</t>
         </is>
       </c>
-      <c r="B815" t="inlineStr">
-        <is>
-          <t>3410</t>
-        </is>
-      </c>
-      <c r="C815" t="inlineStr">
-        <is>
-          <t>333</t>
-        </is>
+      <c r="B815" t="n">
+        <v>3410</v>
+      </c>
+      <c r="C815" t="n">
+        <v>333</v>
       </c>
     </row>
     <row r="816">
@@ -11054,15 +11038,11 @@
           <t>14/05/2025</t>
         </is>
       </c>
-      <c r="B816" t="inlineStr">
-        <is>
-          <t>3760</t>
-        </is>
-      </c>
-      <c r="C816" t="inlineStr">
-        <is>
-          <t>273</t>
-        </is>
+      <c r="B816" t="n">
+        <v>3760</v>
+      </c>
+      <c r="C816" t="n">
+        <v>273</v>
       </c>
     </row>
     <row r="817">
@@ -11071,15 +11051,11 @@
           <t>14/05/2025</t>
         </is>
       </c>
-      <c r="B817" t="inlineStr">
-        <is>
-          <t>3631</t>
-        </is>
-      </c>
-      <c r="C817" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="B817" t="n">
+        <v>3631</v>
+      </c>
+      <c r="C817" t="n">
+        <v>201</v>
       </c>
     </row>
     <row r="818">
@@ -11088,15 +11064,11 @@
           <t>14/05/2025</t>
         </is>
       </c>
-      <c r="B818" t="inlineStr">
-        <is>
-          <t>3630</t>
-        </is>
-      </c>
-      <c r="C818" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="B818" t="n">
+        <v>3630</v>
+      </c>
+      <c r="C818" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="819">
@@ -11105,15 +11077,11 @@
           <t>14/05/2025</t>
         </is>
       </c>
-      <c r="B819" t="inlineStr">
-        <is>
-          <t>3761</t>
-        </is>
-      </c>
-      <c r="C819" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="B819" t="n">
+        <v>3761</v>
+      </c>
+      <c r="C819" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="820">
@@ -11122,15 +11090,11 @@
           <t>14/05/2025</t>
         </is>
       </c>
-      <c r="B820" t="inlineStr">
-        <is>
-          <t>3591</t>
-        </is>
-      </c>
-      <c r="C820" t="inlineStr">
-        <is>
-          <t>51</t>
-        </is>
+      <c r="B820" t="n">
+        <v>3591</v>
+      </c>
+      <c r="C820" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="821">
@@ -11139,15 +11103,11 @@
           <t>14/05/2025</t>
         </is>
       </c>
-      <c r="B821" t="inlineStr">
-        <is>
-          <t>3752</t>
-        </is>
-      </c>
-      <c r="C821" t="inlineStr">
-        <is>
-          <t>69</t>
-        </is>
+      <c r="B821" t="n">
+        <v>3752</v>
+      </c>
+      <c r="C821" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="822">
@@ -11156,14 +11116,769 @@
           <t>14/05/2025</t>
         </is>
       </c>
-      <c r="B822" t="inlineStr">
+      <c r="B822" t="n">
+        <v>3771</v>
+      </c>
+      <c r="C822" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="B823" t="n">
+        <v>2811</v>
+      </c>
+      <c r="C823" t="n">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="B824" t="n">
+        <v>3581</v>
+      </c>
+      <c r="C824" t="n">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="B825" t="n">
+        <v>2651</v>
+      </c>
+      <c r="C825" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="B826" t="n">
+        <v>3410</v>
+      </c>
+      <c r="C826" t="n">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="B827" t="n">
+        <v>3760</v>
+      </c>
+      <c r="C827" t="n">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="B828" t="n">
+        <v>3631</v>
+      </c>
+      <c r="C828" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="B829" t="n">
+        <v>3630</v>
+      </c>
+      <c r="C829" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="B830" t="n">
+        <v>3761</v>
+      </c>
+      <c r="C830" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="B831" t="n">
+        <v>3591</v>
+      </c>
+      <c r="C831" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="B832" t="n">
+        <v>3752</v>
+      </c>
+      <c r="C832" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>14/05/2025</t>
+        </is>
+      </c>
+      <c r="B833" t="n">
+        <v>3771</v>
+      </c>
+      <c r="C833" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="B834" t="n">
+        <v>3410</v>
+      </c>
+      <c r="C834" t="n">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="B835" t="n">
+        <v>3631</v>
+      </c>
+      <c r="C835" t="n">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="B836" t="n">
+        <v>3760</v>
+      </c>
+      <c r="C836" t="n">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="B837" t="n">
+        <v>3581</v>
+      </c>
+      <c r="C837" t="n">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="B838" t="n">
+        <v>2651</v>
+      </c>
+      <c r="C838" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="B839" t="n">
+        <v>2811</v>
+      </c>
+      <c r="C839" t="n">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="B840" t="n">
+        <v>3630</v>
+      </c>
+      <c r="C840" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="B841" t="n">
+        <v>3761</v>
+      </c>
+      <c r="C841" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="B842" t="n">
+        <v>3591</v>
+      </c>
+      <c r="C842" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="B843" t="n">
+        <v>3771</v>
+      </c>
+      <c r="C843" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>15/05/2025</t>
+        </is>
+      </c>
+      <c r="B844" t="n">
+        <v>3752</v>
+      </c>
+      <c r="C844" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>16/05/2025</t>
+        </is>
+      </c>
+      <c r="B845" t="n">
+        <v>3410</v>
+      </c>
+      <c r="C845" t="n">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>16/05/2025</t>
+        </is>
+      </c>
+      <c r="B846" t="n">
+        <v>2651</v>
+      </c>
+      <c r="C846" t="n">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>16/05/2025</t>
+        </is>
+      </c>
+      <c r="B847" t="n">
+        <v>3761</v>
+      </c>
+      <c r="C847" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>16/05/2025</t>
+        </is>
+      </c>
+      <c r="B848" t="n">
+        <v>3760</v>
+      </c>
+      <c r="C848" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>16/05/2025</t>
+        </is>
+      </c>
+      <c r="B849" t="n">
+        <v>3581</v>
+      </c>
+      <c r="C849" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>16/05/2025</t>
+        </is>
+      </c>
+      <c r="B850" t="n">
+        <v>3630</v>
+      </c>
+      <c r="C850" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>16/05/2025</t>
+        </is>
+      </c>
+      <c r="B851" t="n">
+        <v>2811</v>
+      </c>
+      <c r="C851" t="n">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>16/05/2025</t>
+        </is>
+      </c>
+      <c r="B852" t="n">
+        <v>3631</v>
+      </c>
+      <c r="C852" t="n">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>16/05/2025</t>
+        </is>
+      </c>
+      <c r="B853" t="n">
+        <v>3591</v>
+      </c>
+      <c r="C853" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>16/05/2025</t>
+        </is>
+      </c>
+      <c r="B854" t="n">
+        <v>3771</v>
+      </c>
+      <c r="C854" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>16/05/2025</t>
+        </is>
+      </c>
+      <c r="B855" t="n">
+        <v>3752</v>
+      </c>
+      <c r="C855" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
+      </c>
+      <c r="B856" t="n">
+        <v>3760</v>
+      </c>
+      <c r="C856" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
+      </c>
+      <c r="B857" t="n">
+        <v>3410</v>
+      </c>
+      <c r="C857" t="n">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
+      </c>
+      <c r="B858" t="n">
+        <v>2811</v>
+      </c>
+      <c r="C858" t="n">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
+      </c>
+      <c r="B859" t="n">
+        <v>3581</v>
+      </c>
+      <c r="C859" t="n">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
+      </c>
+      <c r="B860" t="n">
+        <v>3761</v>
+      </c>
+      <c r="C860" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
+      </c>
+      <c r="B861" t="n">
+        <v>2651</v>
+      </c>
+      <c r="C861" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
+      </c>
+      <c r="B862" t="n">
+        <v>3630</v>
+      </c>
+      <c r="C862" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
+      </c>
+      <c r="B863" t="n">
+        <v>3631</v>
+      </c>
+      <c r="C863" t="n">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
+      </c>
+      <c r="B864" t="n">
+        <v>3591</v>
+      </c>
+      <c r="C864" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
+      </c>
+      <c r="B865" t="n">
+        <v>3752</v>
+      </c>
+      <c r="C865" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>17/05/2025</t>
+        </is>
+      </c>
+      <c r="B866" t="n">
+        <v>3771</v>
+      </c>
+      <c r="C866" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>2651</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>2811</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>724</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>3410</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>367</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>3581</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>355</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>3761</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>3631</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>214</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>3630</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>3760</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>3591</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
         <is>
           <t>3771</t>
         </is>
       </c>
-      <c r="C822" t="inlineStr">
-        <is>
-          <t>58</t>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>19/05/2025</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>3752</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>14</t>
         </is>
       </c>
     </row>

</xml_diff>